<commit_message>
Fix Carrot coefficients again
</commit_message>
<xml_diff>
--- a/SVSModel/Data/Observed crop parameters.xlsx
+++ b/SVSModel/Data/Observed crop parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\SVSModel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51137B8E-2F47-4D7E-BDD1-E05C04170836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9400FAE-DE7D-4398-BC98-7B5D62BF970A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{37406713-49B3-44B1-928C-6EC17998D6B7}"/>
   </bookViews>
@@ -742,7 +742,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,12 +763,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1223,16 +1217,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91453227-9FB7-42F0-8C4A-4B424D6C8830}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:R503"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="K393" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="K92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E393" sqref="E393"/>
+      <selection pane="bottomRight" activeCell="N398" sqref="N398:N400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,7 +1299,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1346,7 +1340,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1387,7 +1381,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1428,7 +1422,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1463,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1510,7 +1504,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1551,7 +1545,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1592,7 +1586,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1633,7 +1627,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1674,7 +1668,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1715,7 +1709,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1756,7 +1750,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1797,7 +1791,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1838,7 +1832,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1879,7 +1873,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1920,7 +1914,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1961,7 +1955,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -2002,7 +1996,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -2043,7 +2037,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2084,7 +2078,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -2125,7 +2119,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -2166,7 +2160,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2207,7 +2201,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -2248,7 +2242,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2283,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -2330,7 +2324,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -2371,7 +2365,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -2412,7 +2406,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2453,7 +2447,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -2494,7 +2488,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -2535,7 +2529,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -2576,7 +2570,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2617,7 +2611,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -2658,7 +2652,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -2699,7 +2693,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -2740,7 +2734,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2781,7 +2775,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -2822,7 +2816,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -2863,7 +2857,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -2904,7 +2898,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -2945,7 +2939,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -2986,7 +2980,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -3027,7 +3021,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -3068,7 +3062,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -3109,7 +3103,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -3150,7 +3144,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -3191,7 +3185,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -3232,7 +3226,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -3273,7 +3267,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -3314,7 +3308,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -3355,7 +3349,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -3396,7 +3390,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -3437,7 +3431,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -3478,7 +3472,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -3519,7 +3513,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -3560,7 +3554,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -3601,7 +3595,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -3642,7 +3636,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -3683,7 +3677,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -3724,7 +3718,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -3765,7 +3759,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -3806,7 +3800,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -3847,7 +3841,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -3888,7 +3882,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -3929,7 +3923,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -3970,7 +3964,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -4011,7 +4005,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -4052,7 +4046,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -4093,7 +4087,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4128,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -4175,7 +4169,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -4216,7 +4210,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -4257,7 +4251,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
@@ -4298,7 +4292,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -4339,7 +4333,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -4380,7 +4374,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -4421,7 +4415,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -4462,7 +4456,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -4503,7 +4497,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -4544,7 +4538,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -4585,7 +4579,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
@@ -4626,7 +4620,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
@@ -4667,7 +4661,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -4708,7 +4702,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
@@ -4749,7 +4743,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -4790,7 +4784,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -4831,7 +4825,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
@@ -4872,7 +4866,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
@@ -4913,7 +4907,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -4954,7 +4948,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>0</v>
       </c>
@@ -5005,8 +4999,8 @@
       <c r="D92" t="s">
         <v>17</v>
       </c>
-      <c r="E92" t="s">
-        <v>18</v>
+      <c r="E92" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="F92">
         <v>31</v>
@@ -5046,8 +5040,8 @@
       <c r="D93" t="s">
         <v>17</v>
       </c>
-      <c r="E93" t="s">
-        <v>18</v>
+      <c r="E93" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="F93">
         <v>31</v>
@@ -5087,8 +5081,8 @@
       <c r="D94" t="s">
         <v>17</v>
       </c>
-      <c r="E94" t="s">
-        <v>18</v>
+      <c r="E94" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="F94">
         <v>31</v>
@@ -5128,8 +5122,8 @@
       <c r="D95" t="s">
         <v>17</v>
       </c>
-      <c r="E95" t="s">
-        <v>18</v>
+      <c r="E95" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="F95">
         <v>32</v>
@@ -5169,8 +5163,8 @@
       <c r="D96" t="s">
         <v>17</v>
       </c>
-      <c r="E96" t="s">
-        <v>18</v>
+      <c r="E96" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="F96">
         <v>32</v>
@@ -5210,8 +5204,8 @@
       <c r="D97" t="s">
         <v>17</v>
       </c>
-      <c r="E97" t="s">
-        <v>18</v>
+      <c r="E97" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="F97">
         <v>32</v>
@@ -5241,7 +5235,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>0</v>
       </c>
@@ -5282,7 +5276,7 @@
         <v>0.31111111111111112</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>0</v>
       </c>
@@ -5323,7 +5317,7 @@
         <v>0.49777777777777787</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -5364,7 +5358,7 @@
         <v>0.3166666666666666</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -5405,7 +5399,7 @@
         <v>0.29699999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
@@ -5446,7 +5440,7 @@
         <v>0.19083333333333333</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -5487,7 +5481,7 @@
         <v>0.21812500000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>0</v>
       </c>
@@ -5528,7 +5522,7 @@
         <v>0.23777777777777778</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>0</v>
       </c>
@@ -5569,7 +5563,7 @@
         <v>0.176875</v>
       </c>
     </row>
-    <row r="106" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="20" t="s">
         <v>0</v>
       </c>
@@ -5603,7 +5597,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>0</v>
       </c>
@@ -5644,7 +5638,7 @@
         <v>0.25249999999999995</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>0</v>
       </c>
@@ -5685,7 +5679,7 @@
         <v>0.28533333333333333</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>0</v>
       </c>
@@ -5726,7 +5720,7 @@
         <v>0.21466666666666667</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>0</v>
       </c>
@@ -5767,7 +5761,7 @@
         <v>0.25680000000000003</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>0</v>
       </c>
@@ -5808,7 +5802,7 @@
         <v>0.27318181818181819</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>0</v>
       </c>
@@ -5849,7 +5843,7 @@
         <v>0.28260869565217389</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>0</v>
       </c>
@@ -5890,7 +5884,7 @@
         <v>0.34166666666666667</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
@@ -5931,7 +5925,7 @@
         <v>0.25377358490566038</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>0</v>
       </c>
@@ -5972,7 +5966,7 @@
         <v>0.315</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>0</v>
       </c>
@@ -6013,7 +6007,7 @@
         <v>4.2965517241379314E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>0</v>
       </c>
@@ -6054,7 +6048,7 @@
         <v>5.9607142857142852E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>0</v>
       </c>
@@ -6095,7 +6089,7 @@
         <v>5.4999999999999993E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>0</v>
       </c>
@@ -6136,7 +6130,7 @@
         <v>0.4885714285714286</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>0</v>
       </c>
@@ -6177,7 +6171,7 @@
         <v>0.51647058823529413</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>0</v>
       </c>
@@ -6218,7 +6212,7 @@
         <v>0.49647058823529416</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>0</v>
       </c>
@@ -6262,7 +6256,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>0</v>
       </c>
@@ -6306,7 +6300,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>0</v>
       </c>
@@ -6350,7 +6344,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="125" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>0</v>
       </c>
@@ -6396,7 +6390,7 @@
       </c>
       <c r="R125" s="6"/>
     </row>
-    <row r="126" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>0</v>
       </c>
@@ -6442,7 +6436,7 @@
       </c>
       <c r="R126" s="6"/>
     </row>
-    <row r="127" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>0</v>
       </c>
@@ -6488,7 +6482,7 @@
       </c>
       <c r="R127" s="6"/>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>0</v>
       </c>
@@ -6529,7 +6523,7 @@
         <v>0.27875</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>0</v>
       </c>
@@ -6570,7 +6564,7 @@
         <v>0.27241379310344832</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>0</v>
       </c>
@@ -6611,7 +6605,7 @@
         <v>0.26096153846153847</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>0</v>
       </c>
@@ -6652,7 +6646,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>0</v>
       </c>
@@ -6693,7 +6687,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
@@ -6734,7 +6728,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>0</v>
       </c>
@@ -6775,7 +6769,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>0</v>
       </c>
@@ -6816,7 +6810,7 @@
         <v>0.52187499999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>0</v>
       </c>
@@ -6857,7 +6851,7 @@
         <v>0.56937500000000008</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>0</v>
       </c>
@@ -6898,7 +6892,7 @@
         <v>0.71000000000000008</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>0</v>
       </c>
@@ -6939,7 +6933,7 @@
         <v>0.68562500000000004</v>
       </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>0</v>
       </c>
@@ -6980,7 +6974,7 @@
         <v>0.57125000000000004</v>
       </c>
     </row>
-    <row r="140" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>0</v>
       </c>
@@ -7026,7 +7020,7 @@
       </c>
       <c r="R140" s="6"/>
     </row>
-    <row r="141" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>0</v>
       </c>
@@ -7072,7 +7066,7 @@
       </c>
       <c r="R141" s="6"/>
     </row>
-    <row r="142" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="20" t="s">
         <v>0</v>
       </c>
@@ -7106,7 +7100,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>0</v>
       </c>
@@ -7147,7 +7141,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>0</v>
       </c>
@@ -7188,7 +7182,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>0</v>
       </c>
@@ -7229,7 +7223,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>0</v>
       </c>
@@ -7267,7 +7261,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>0</v>
       </c>
@@ -7305,7 +7299,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>0</v>
       </c>
@@ -7343,7 +7337,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="20" t="s">
         <v>0</v>
       </c>
@@ -7377,7 +7371,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="150" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="20" t="s">
         <v>0</v>
       </c>
@@ -7411,7 +7405,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="151" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="20" t="s">
         <v>0</v>
       </c>
@@ -7445,7 +7439,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>0</v>
       </c>
@@ -7486,7 +7480,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>0</v>
       </c>
@@ -7527,7 +7521,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="154" spans="1:18" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:18" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>0</v>
       </c>
@@ -7573,7 +7567,7 @@
       </c>
       <c r="R154" s="6"/>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>0</v>
       </c>
@@ -7614,7 +7608,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>0</v>
       </c>
@@ -7655,7 +7649,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>0</v>
       </c>
@@ -7696,7 +7690,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>0</v>
       </c>
@@ -7737,7 +7731,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>0</v>
       </c>
@@ -7778,7 +7772,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>0</v>
       </c>
@@ -7819,7 +7813,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>0</v>
       </c>
@@ -7860,7 +7854,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>0</v>
       </c>
@@ -7901,7 +7895,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>0</v>
       </c>
@@ -7942,7 +7936,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>0</v>
       </c>
@@ -7983,7 +7977,7 @@
         <v>5.7167381974248935E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>0</v>
       </c>
@@ -8024,7 +8018,7 @@
         <v>6.2093023255813957E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:18" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="s">
         <v>0</v>
       </c>
@@ -8070,7 +8064,7 @@
       </c>
       <c r="R166" s="7"/>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>65</v>
       </c>
@@ -8111,7 +8105,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>65</v>
       </c>
@@ -8152,7 +8146,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>65</v>
       </c>
@@ -8193,7 +8187,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>65</v>
       </c>
@@ -8234,7 +8228,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>65</v>
       </c>
@@ -8275,7 +8269,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>65</v>
       </c>
@@ -8316,7 +8310,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>65</v>
       </c>
@@ -8357,7 +8351,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>65</v>
       </c>
@@ -8398,7 +8392,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>65</v>
       </c>
@@ -8439,7 +8433,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>65</v>
       </c>
@@ -8480,7 +8474,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>65</v>
       </c>
@@ -8521,7 +8515,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>65</v>
       </c>
@@ -8562,7 +8556,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>65</v>
       </c>
@@ -8603,7 +8597,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>65</v>
       </c>
@@ -8644,7 +8638,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>65</v>
       </c>
@@ -8685,7 +8679,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>65</v>
       </c>
@@ -8726,7 +8720,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>65</v>
       </c>
@@ -8764,7 +8758,7 @@
         <v>0.25333555900621119</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>65</v>
       </c>
@@ -8802,7 +8796,7 @@
         <v>0.24928007723112128</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>65</v>
       </c>
@@ -8840,7 +8834,7 @@
         <v>0.24416219179371351</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>65</v>
       </c>
@@ -8878,7 +8872,7 @@
         <v>0.2797665909090909</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>65</v>
       </c>
@@ -8916,7 +8910,7 @@
         <v>0.20726497826086956</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>65</v>
       </c>
@@ -8954,7 +8948,7 @@
         <v>0.2255453409090909</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>65</v>
       </c>
@@ -8992,7 +8986,7 @@
         <v>0.28862180735930737</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>65</v>
       </c>
@@ -9030,7 +9024,7 @@
         <v>0.27043159937888195</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>65</v>
       </c>
@@ -9068,7 +9062,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>65</v>
       </c>
@@ -9106,7 +9100,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>65</v>
       </c>
@@ -9144,7 +9138,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>65</v>
       </c>
@@ -9182,7 +9176,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>65</v>
       </c>
@@ -9220,7 +9214,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>65</v>
       </c>
@@ -9258,7 +9252,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>65</v>
       </c>
@@ -9299,7 +9293,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>65</v>
       </c>
@@ -9337,7 +9331,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>65</v>
       </c>
@@ -9378,7 +9372,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>65</v>
       </c>
@@ -9419,7 +9413,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>65</v>
       </c>
@@ -9460,7 +9454,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>65</v>
       </c>
@@ -9501,7 +9495,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>65</v>
       </c>
@@ -9542,7 +9536,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>65</v>
       </c>
@@ -9583,7 +9577,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>65</v>
       </c>
@@ -9624,7 +9618,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>65</v>
       </c>
@@ -9665,7 +9659,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>65</v>
       </c>
@@ -9703,7 +9697,7 @@
         <v>7.2216898987798039E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>65</v>
       </c>
@@ -9741,7 +9735,7 @@
         <v>7.0520640901221288E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>65</v>
       </c>
@@ -9779,7 +9773,7 @@
         <v>7.349693974535873E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>65</v>
       </c>
@@ -9817,7 +9811,7 @@
         <v>8.7933980879310591E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>65</v>
       </c>
@@ -9855,7 +9849,7 @@
         <v>7.0796834573684742E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>65</v>
       </c>
@@ -9893,7 +9887,7 @@
         <v>7.8219417007123329E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>65</v>
       </c>
@@ -9931,7 +9925,7 @@
         <v>8.2617036957847445E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>65</v>
       </c>
@@ -9969,7 +9963,7 @@
         <v>9.0979325992371518E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>65</v>
       </c>
@@ -10007,7 +10001,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>65</v>
       </c>
@@ -10045,7 +10039,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>65</v>
       </c>
@@ -10083,7 +10077,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>65</v>
       </c>
@@ -10121,7 +10115,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>65</v>
       </c>
@@ -10159,7 +10153,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>65</v>
       </c>
@@ -10197,7 +10191,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>65</v>
       </c>
@@ -10235,7 +10229,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>65</v>
       </c>
@@ -10273,7 +10267,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>65</v>
       </c>
@@ -10311,7 +10305,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>65</v>
       </c>
@@ -10349,7 +10343,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>65</v>
       </c>
@@ -10387,7 +10381,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>65</v>
       </c>
@@ -10425,7 +10419,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>65</v>
       </c>
@@ -10463,7 +10457,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>65</v>
       </c>
@@ -10501,7 +10495,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>65</v>
       </c>
@@ -10539,7 +10533,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>65</v>
       </c>
@@ -10577,7 +10571,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>65</v>
       </c>
@@ -10618,7 +10612,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>65</v>
       </c>
@@ -10659,7 +10653,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>65</v>
       </c>
@@ -10700,7 +10694,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>65</v>
       </c>
@@ -10741,7 +10735,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>65</v>
       </c>
@@ -10782,7 +10776,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="236" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>65</v>
       </c>
@@ -10823,7 +10817,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>65</v>
       </c>
@@ -10864,7 +10858,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>65</v>
       </c>
@@ -10905,7 +10899,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>65</v>
       </c>
@@ -10943,7 +10937,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>65</v>
       </c>
@@ -10981,7 +10975,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>65</v>
       </c>
@@ -11019,7 +11013,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>65</v>
       </c>
@@ -11057,7 +11051,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>65</v>
       </c>
@@ -11095,7 +11089,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>65</v>
       </c>
@@ -11133,7 +11127,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>65</v>
       </c>
@@ -11171,7 +11165,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>65</v>
       </c>
@@ -11209,7 +11203,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>65</v>
       </c>
@@ -11247,7 +11241,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>65</v>
       </c>
@@ -11285,7 +11279,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>65</v>
       </c>
@@ -11323,7 +11317,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>65</v>
       </c>
@@ -11361,7 +11355,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>65</v>
       </c>
@@ -11399,7 +11393,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>65</v>
       </c>
@@ -11437,7 +11431,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>65</v>
       </c>
@@ -11475,7 +11469,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>65</v>
       </c>
@@ -11513,7 +11507,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>65</v>
       </c>
@@ -11551,7 +11545,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>65</v>
       </c>
@@ -11589,7 +11583,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>65</v>
       </c>
@@ -11627,7 +11621,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>65</v>
       </c>
@@ -11665,7 +11659,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>65</v>
       </c>
@@ -11703,7 +11697,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>65</v>
       </c>
@@ -11741,7 +11735,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>65</v>
       </c>
@@ -11779,7 +11773,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>65</v>
       </c>
@@ -11817,7 +11811,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>65</v>
       </c>
@@ -11855,7 +11849,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>65</v>
       </c>
@@ -11893,7 +11887,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>65</v>
       </c>
@@ -11931,7 +11925,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>65</v>
       </c>
@@ -11969,7 +11963,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>65</v>
       </c>
@@ -12007,7 +12001,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>65</v>
       </c>
@@ -12045,7 +12039,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>65</v>
       </c>
@@ -12083,7 +12077,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>65</v>
       </c>
@@ -12121,7 +12115,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>65</v>
       </c>
@@ -12159,7 +12153,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>65</v>
       </c>
@@ -12197,7 +12191,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="273" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>65</v>
       </c>
@@ -12235,7 +12229,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="274" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>65</v>
       </c>
@@ -12273,7 +12267,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="275" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
         <v>65</v>
       </c>
@@ -12311,7 +12305,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="276" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>65</v>
       </c>
@@ -12349,7 +12343,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="277" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
         <v>65</v>
       </c>
@@ -12387,7 +12381,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="278" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>65</v>
       </c>
@@ -12425,7 +12419,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="279" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>65</v>
       </c>
@@ -12463,7 +12457,7 @@
         <v>7.3597288810245354E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
         <v>65</v>
       </c>
@@ -12501,7 +12495,7 @@
         <v>7.7729074376716278E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>65</v>
       </c>
@@ -12539,7 +12533,7 @@
         <v>7.1837560890749302E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>65</v>
       </c>
@@ -12577,7 +12571,7 @@
         <v>8.775434774157824E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
         <v>65</v>
       </c>
@@ -12615,7 +12609,7 @@
         <v>7.2161903550698181E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>65</v>
       </c>
@@ -12653,7 +12647,7 @@
         <v>6.5504538315512506E-2</v>
       </c>
     </row>
-    <row r="285" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>65</v>
       </c>
@@ -12691,7 +12685,7 @@
         <v>6.8494839348744799E-2</v>
       </c>
     </row>
-    <row r="286" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>65</v>
       </c>
@@ -12729,7 +12723,7 @@
         <v>6.9433278727134728E-2</v>
       </c>
     </row>
-    <row r="287" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>65</v>
       </c>
@@ -12770,7 +12764,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="288" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>65</v>
       </c>
@@ -12811,7 +12805,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="289" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
         <v>65</v>
       </c>
@@ -12852,7 +12846,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="290" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>65</v>
       </c>
@@ -12893,7 +12887,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="291" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>65</v>
       </c>
@@ -12934,7 +12928,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="292" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>65</v>
       </c>
@@ -12975,7 +12969,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="293" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>65</v>
       </c>
@@ -13016,7 +13010,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="294" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>65</v>
       </c>
@@ -13057,7 +13051,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="295" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>65</v>
       </c>
@@ -13098,7 +13092,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="296" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>65</v>
       </c>
@@ -13139,7 +13133,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="297" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
         <v>65</v>
       </c>
@@ -13180,7 +13174,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="298" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
         <v>65</v>
       </c>
@@ -13221,7 +13215,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="299" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
         <v>65</v>
       </c>
@@ -13262,7 +13256,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="300" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>65</v>
       </c>
@@ -13303,7 +13297,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="301" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
         <v>65</v>
       </c>
@@ -13344,7 +13338,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="302" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
         <v>65</v>
       </c>
@@ -13385,7 +13379,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="303" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>65</v>
       </c>
@@ -13426,7 +13420,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="304" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
         <v>65</v>
       </c>
@@ -13467,7 +13461,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="305" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
         <v>65</v>
       </c>
@@ -13508,7 +13502,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="306" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
         <v>65</v>
       </c>
@@ -13549,7 +13543,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="307" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>65</v>
       </c>
@@ -13590,7 +13584,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="308" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
         <v>65</v>
       </c>
@@ -13631,7 +13625,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="309" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
         <v>65</v>
       </c>
@@ -13672,7 +13666,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="310" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
         <v>65</v>
       </c>
@@ -13713,7 +13707,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="311" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
         <v>65</v>
       </c>
@@ -13754,7 +13748,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="312" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
         <v>65</v>
       </c>
@@ -13795,7 +13789,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="313" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
         <v>65</v>
       </c>
@@ -13836,7 +13830,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="314" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
         <v>65</v>
       </c>
@@ -13877,7 +13871,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="315" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
         <v>65</v>
       </c>
@@ -13918,7 +13912,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="316" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
         <v>65</v>
       </c>
@@ -13959,7 +13953,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="317" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
         <v>65</v>
       </c>
@@ -14000,7 +13994,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="318" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
         <v>65</v>
       </c>
@@ -14041,7 +14035,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="319" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
         <v>65</v>
       </c>
@@ -14082,7 +14076,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="320" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
         <v>65</v>
       </c>
@@ -14123,7 +14117,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="321" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
         <v>65</v>
       </c>
@@ -14164,7 +14158,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="322" spans="1:18" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:18" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A322" s="1" t="s">
         <v>65</v>
       </c>
@@ -14210,7 +14204,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="323" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
         <v>65</v>
       </c>
@@ -14251,7 +14245,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="324" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
         <v>65</v>
       </c>
@@ -14292,7 +14286,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="325" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
         <v>65</v>
       </c>
@@ -14333,7 +14327,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="326" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
         <v>65</v>
       </c>
@@ -14374,7 +14368,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="327" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
         <v>65</v>
       </c>
@@ -14415,7 +14409,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="328" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
         <v>65</v>
       </c>
@@ -14456,7 +14450,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="329" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
         <v>65</v>
       </c>
@@ -14497,7 +14491,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="330" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
         <v>65</v>
       </c>
@@ -14538,7 +14532,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="331" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
         <v>65</v>
       </c>
@@ -14579,7 +14573,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="332" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
         <v>65</v>
       </c>
@@ -14620,7 +14614,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="333" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
         <v>65</v>
       </c>
@@ -14661,7 +14655,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="334" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:18" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A334" s="3" t="s">
         <v>65</v>
       </c>
@@ -14707,7 +14701,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="335" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" s="15" t="s">
         <v>90</v>
       </c>
@@ -14749,7 +14743,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="336" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" s="15" t="s">
         <v>90</v>
       </c>
@@ -14791,7 +14785,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" s="15" t="s">
         <v>90</v>
       </c>
@@ -14833,7 +14827,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" s="15" t="s">
         <v>90</v>
       </c>
@@ -14875,7 +14869,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" s="15" t="s">
         <v>90</v>
       </c>
@@ -14917,7 +14911,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" s="15" t="s">
         <v>90</v>
       </c>
@@ -14959,7 +14953,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" s="15" t="s">
         <v>90</v>
       </c>
@@ -14998,7 +14992,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" s="15" t="s">
         <v>90</v>
       </c>
@@ -15037,7 +15031,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" s="15" t="s">
         <v>90</v>
       </c>
@@ -15076,7 +15070,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" s="15" t="s">
         <v>90</v>
       </c>
@@ -15118,7 +15112,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" s="15" t="s">
         <v>90</v>
       </c>
@@ -15160,7 +15154,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" s="15" t="s">
         <v>90</v>
       </c>
@@ -15202,7 +15196,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" s="15" t="s">
         <v>90</v>
       </c>
@@ -15244,7 +15238,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" s="15" t="s">
         <v>90</v>
       </c>
@@ -15286,7 +15280,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" s="15" t="s">
         <v>90</v>
       </c>
@@ -15328,7 +15322,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" s="15" t="s">
         <v>90</v>
       </c>
@@ -15370,7 +15364,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" s="15" t="s">
         <v>90</v>
       </c>
@@ -15412,7 +15406,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" s="15" t="s">
         <v>90</v>
       </c>
@@ -15454,7 +15448,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="353" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" s="15" t="s">
         <v>90</v>
       </c>
@@ -15496,7 +15490,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="354" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" s="15" t="s">
         <v>90</v>
       </c>
@@ -15538,7 +15532,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="355" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" s="15" t="s">
         <v>90</v>
       </c>
@@ -15580,7 +15574,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="356" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" s="15" t="s">
         <v>90</v>
       </c>
@@ -15622,7 +15616,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="357" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" s="15" t="s">
         <v>90</v>
       </c>
@@ -15664,7 +15658,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="358" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" s="15" t="s">
         <v>90</v>
       </c>
@@ -15706,7 +15700,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="359" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" s="15" t="s">
         <v>90</v>
       </c>
@@ -15748,7 +15742,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="360" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" s="15" t="s">
         <v>90</v>
       </c>
@@ -15790,7 +15784,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="361" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" s="15" t="s">
         <v>90</v>
       </c>
@@ -15832,7 +15826,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="362" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" s="15" t="s">
         <v>90</v>
       </c>
@@ -15878,7 +15872,7 @@
       </c>
       <c r="R362" s="6"/>
     </row>
-    <row r="363" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" s="15" t="s">
         <v>90</v>
       </c>
@@ -15924,7 +15918,7 @@
       </c>
       <c r="R363" s="6"/>
     </row>
-    <row r="364" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" s="15" t="s">
         <v>90</v>
       </c>
@@ -15970,7 +15964,7 @@
       </c>
       <c r="R364" s="6"/>
     </row>
-    <row r="365" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" s="15" t="s">
         <v>90</v>
       </c>
@@ -16016,7 +16010,7 @@
       </c>
       <c r="R365" s="6"/>
     </row>
-    <row r="366" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" s="15" t="s">
         <v>90</v>
       </c>
@@ -16062,7 +16056,7 @@
       </c>
       <c r="R366" s="6"/>
     </row>
-    <row r="367" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367" s="15" t="s">
         <v>90</v>
       </c>
@@ -16108,7 +16102,7 @@
       </c>
       <c r="R367" s="6"/>
     </row>
-    <row r="368" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" s="15" t="s">
         <v>90</v>
       </c>
@@ -16154,7 +16148,7 @@
       </c>
       <c r="R368" s="6"/>
     </row>
-    <row r="369" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A369" s="15" t="s">
         <v>90</v>
       </c>
@@ -16200,7 +16194,7 @@
       </c>
       <c r="R369" s="6"/>
     </row>
-    <row r="370" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" s="15" t="s">
         <v>90</v>
       </c>
@@ -16246,7 +16240,7 @@
       </c>
       <c r="R370" s="6"/>
     </row>
-    <row r="371" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" s="15" t="s">
         <v>90</v>
       </c>
@@ -16292,7 +16286,7 @@
       </c>
       <c r="R371" s="6"/>
     </row>
-    <row r="372" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" s="15" t="s">
         <v>90</v>
       </c>
@@ -16334,7 +16328,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="373" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" s="15" t="s">
         <v>90</v>
       </c>
@@ -16376,7 +16370,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="374" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A374" s="15" t="s">
         <v>90</v>
       </c>
@@ -16418,7 +16412,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="375" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" s="15" t="s">
         <v>90</v>
       </c>
@@ -16464,7 +16458,7 @@
       </c>
       <c r="R375" s="6"/>
     </row>
-    <row r="376" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A376" s="15" t="s">
         <v>90</v>
       </c>
@@ -16506,7 +16500,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="377" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" s="15" t="s">
         <v>90</v>
       </c>
@@ -16548,7 +16542,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="378" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378" s="15" t="s">
         <v>90</v>
       </c>
@@ -16590,7 +16584,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="379" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" s="17" t="s">
         <v>90</v>
       </c>
@@ -16622,7 +16616,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="380" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" s="17" t="s">
         <v>90</v>
       </c>
@@ -16654,7 +16648,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="381" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A381" s="17" t="s">
         <v>90</v>
       </c>
@@ -16686,7 +16680,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="382" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A382" s="17" t="s">
         <v>90</v>
       </c>
@@ -16718,7 +16712,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="383" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383" s="17" t="s">
         <v>90</v>
       </c>
@@ -16750,7 +16744,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="384" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384" s="15" t="s">
         <v>90</v>
       </c>
@@ -16789,7 +16783,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="385" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385" s="15" t="s">
         <v>90</v>
       </c>
@@ -16828,7 +16822,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="386" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" s="15" t="s">
         <v>90</v>
       </c>
@@ -16867,7 +16861,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="387" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387" s="17" t="s">
         <v>90</v>
       </c>
@@ -16899,7 +16893,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="388" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" s="17" t="s">
         <v>90</v>
       </c>
@@ -16931,7 +16925,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="389" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" s="17" t="s">
         <v>90</v>
       </c>
@@ -16963,7 +16957,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="390" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:18" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A390" s="15" t="s">
         <v>90</v>
       </c>
@@ -17009,7 +17003,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="391" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:18" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A391" s="15" t="s">
         <v>90</v>
       </c>
@@ -17055,7 +17049,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="392" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:18" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" s="15" t="s">
         <v>90</v>
       </c>
@@ -17101,7 +17095,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="393" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" s="15" t="s">
         <v>90</v>
       </c>
@@ -17143,7 +17137,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="394" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" s="15" t="s">
         <v>90</v>
       </c>
@@ -17185,7 +17179,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="395" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A395" s="15" t="s">
         <v>90</v>
       </c>
@@ -17227,7 +17221,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="396" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A396" s="15" t="s">
         <v>90</v>
       </c>
@@ -17269,7 +17263,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="397" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A397" s="15" t="s">
         <v>90</v>
       </c>
@@ -17432,7 +17426,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="401" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A401" s="15" t="s">
         <v>90</v>
       </c>
@@ -17471,7 +17465,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="402" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A402" s="15" t="s">
         <v>90</v>
       </c>
@@ -17510,7 +17504,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="403" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A403" s="15" t="s">
         <v>90</v>
       </c>
@@ -17549,7 +17543,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="404" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" s="17" t="s">
         <v>90</v>
       </c>
@@ -17581,7 +17575,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="405" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" s="17" t="s">
         <v>90</v>
       </c>
@@ -17613,7 +17607,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="406" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A406" s="17" t="s">
         <v>90</v>
       </c>
@@ -17645,7 +17639,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="407" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A407" s="15" t="s">
         <v>90</v>
       </c>
@@ -17684,7 +17678,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="408" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A408" s="15" t="s">
         <v>90</v>
       </c>
@@ -17723,7 +17717,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="409" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A409" s="15" t="s">
         <v>90</v>
       </c>
@@ -17762,7 +17756,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="410" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" s="15" t="s">
         <v>90</v>
       </c>
@@ -17801,7 +17795,7 @@
         <v>0.84599999999999997</v>
       </c>
     </row>
-    <row r="411" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A411" s="17" t="s">
         <v>90</v>
       </c>
@@ -17847,7 +17841,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="412" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A412" s="15" t="s">
         <v>90</v>
       </c>
@@ -17886,7 +17880,7 @@
         <v>0.59000000000000008</v>
       </c>
     </row>
-    <row r="413" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A413" s="15" t="s">
         <v>90</v>
       </c>
@@ -17925,7 +17919,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="414" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A414" s="15" t="s">
         <v>90</v>
       </c>
@@ -17964,7 +17958,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="415" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A415" s="15" t="s">
         <v>90</v>
       </c>
@@ -18003,7 +17997,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="416" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A416" s="15" t="s">
         <v>90</v>
       </c>
@@ -18045,7 +18039,7 @@
       <c r="Q416"/>
       <c r="R416" s="6"/>
     </row>
-    <row r="417" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A417" s="15" t="s">
         <v>90</v>
       </c>
@@ -18087,7 +18081,7 @@
       <c r="Q417"/>
       <c r="R417" s="6"/>
     </row>
-    <row r="418" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A418" s="15" t="s">
         <v>90</v>
       </c>
@@ -18129,7 +18123,7 @@
       <c r="Q418"/>
       <c r="R418" s="6"/>
     </row>
-    <row r="419" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A419" s="15" t="s">
         <v>90</v>
       </c>
@@ -18166,7 +18160,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="420" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A420" s="15" t="s">
         <v>90</v>
       </c>
@@ -18203,7 +18197,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="421" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A421" s="15" t="s">
         <v>90</v>
       </c>
@@ -18240,7 +18234,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="422" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A422" s="15" t="s">
         <v>90</v>
       </c>
@@ -18277,7 +18271,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="423" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A423" s="15" t="s">
         <v>90</v>
       </c>
@@ -18314,7 +18308,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="424" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A424" s="15" t="s">
         <v>90</v>
       </c>
@@ -18350,7 +18344,7 @@
         <v>54638.888888888898</v>
       </c>
     </row>
-    <row r="425" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A425" s="15" t="s">
         <v>90</v>
       </c>
@@ -18386,7 +18380,7 @@
         <v>54638.888888888898</v>
       </c>
     </row>
-    <row r="426" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A426" s="15" t="s">
         <v>90</v>
       </c>
@@ -18422,7 +18416,7 @@
         <v>54638.888888888898</v>
       </c>
     </row>
-    <row r="427" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A427" s="15" t="s">
         <v>90</v>
       </c>
@@ -18464,7 +18458,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="428" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A428" s="15" t="s">
         <v>90</v>
       </c>
@@ -18510,7 +18504,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="429" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A429" s="15" t="s">
         <v>90</v>
       </c>
@@ -18556,7 +18550,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="430" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A430" s="17" t="s">
         <v>90</v>
       </c>
@@ -18588,7 +18582,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="431" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A431" s="17" t="s">
         <v>90</v>
       </c>
@@ -18620,7 +18614,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="432" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A432" s="17" t="s">
         <v>90</v>
       </c>
@@ -18652,7 +18646,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="433" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A433" s="15" t="s">
         <v>90</v>
       </c>
@@ -18694,7 +18688,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="434" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A434" s="15" t="s">
         <v>90</v>
       </c>
@@ -18740,7 +18734,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="435" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A435" s="15" t="s">
         <v>90</v>
       </c>
@@ -18786,7 +18780,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="436" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A436" s="15" t="s">
         <v>90</v>
       </c>
@@ -18830,7 +18824,7 @@
       </c>
       <c r="R436" s="6"/>
     </row>
-    <row r="437" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A437" s="15" t="s">
         <v>90</v>
       </c>
@@ -18869,7 +18863,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="438" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A438" s="15" t="s">
         <v>90</v>
       </c>
@@ -18908,7 +18902,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="439" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A439" s="15" t="s">
         <v>90</v>
       </c>
@@ -18947,7 +18941,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="440" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A440" s="15" t="s">
         <v>90</v>
       </c>
@@ -18991,7 +18985,7 @@
       </c>
       <c r="R440" s="6"/>
     </row>
-    <row r="441" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A441" s="15" t="s">
         <v>90</v>
       </c>
@@ -19035,7 +19029,7 @@
       </c>
       <c r="R441" s="6"/>
     </row>
-    <row r="442" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:18" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A442" s="15" t="s">
         <v>90</v>
       </c>
@@ -19079,7 +19073,7 @@
       </c>
       <c r="R442" s="6"/>
     </row>
-    <row r="443" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:18" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A443" s="15" t="s">
         <v>90</v>
       </c>
@@ -19123,7 +19117,7 @@
       </c>
       <c r="R443" s="6"/>
     </row>
-    <row r="444" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:18" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A444" s="15" t="s">
         <v>90</v>
       </c>
@@ -19167,7 +19161,7 @@
       </c>
       <c r="R444" s="6"/>
     </row>
-    <row r="445" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:18" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A445" s="15" t="s">
         <v>90</v>
       </c>
@@ -19211,7 +19205,7 @@
       </c>
       <c r="R445" s="6"/>
     </row>
-    <row r="446" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A446" s="15" t="s">
         <v>90</v>
       </c>
@@ -19250,7 +19244,7 @@
         <v>1.7640000000000002</v>
       </c>
     </row>
-    <row r="447" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A447" s="15" t="s">
         <v>90</v>
       </c>
@@ -19289,7 +19283,7 @@
         <v>1.6466666666666672</v>
       </c>
     </row>
-    <row r="448" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A448" s="15" t="s">
         <v>90</v>
       </c>
@@ -19331,7 +19325,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="449" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A449" s="15" t="s">
         <v>90</v>
       </c>
@@ -19373,7 +19367,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="450" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A450" s="15" t="s">
         <v>90</v>
       </c>
@@ -19415,7 +19409,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="451" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A451" s="15" t="s">
         <v>90</v>
       </c>
@@ -19454,7 +19448,7 @@
         <v>7.6195833333333338</v>
       </c>
     </row>
-    <row r="452" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A452" s="15" t="s">
         <v>90</v>
       </c>
@@ -19493,7 +19487,7 @@
         <v>7.1081999999999992</v>
       </c>
     </row>
-    <row r="453" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A453" s="15" t="s">
         <v>90</v>
       </c>
@@ -19532,7 +19526,7 @@
         <v>5.1807500000000006</v>
       </c>
     </row>
-    <row r="454" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A454" s="17" t="s">
         <v>90</v>
       </c>
@@ -19564,7 +19558,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="455" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A455" s="17" t="s">
         <v>90</v>
       </c>
@@ -19596,7 +19590,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="456" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A456" s="17" t="s">
         <v>90</v>
       </c>
@@ -19628,7 +19622,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="457" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:18" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A457" s="17" t="s">
         <v>90</v>
       </c>
@@ -19649,7 +19643,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="458" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:18" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A458" s="17" t="s">
         <v>90</v>
       </c>
@@ -19670,7 +19664,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="459" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:18" s="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A459" s="17" t="s">
         <v>90</v>
       </c>
@@ -19691,7 +19685,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="460" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A460" s="15" t="s">
         <v>90</v>
       </c>
@@ -19733,7 +19727,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="461" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A461" s="15" t="s">
         <v>90</v>
       </c>
@@ -19775,7 +19769,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="462" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A462" s="15" t="s">
         <v>90</v>
       </c>
@@ -19817,7 +19811,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="463" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A463" s="15" t="s">
         <v>90</v>
       </c>
@@ -19859,7 +19853,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="464" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A464" s="15" t="s">
         <v>90</v>
       </c>
@@ -19901,7 +19895,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="465" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A465" s="15" t="s">
         <v>90</v>
       </c>
@@ -19940,7 +19934,7 @@
         <v>1.611</v>
       </c>
     </row>
-    <row r="466" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A466" s="15" t="s">
         <v>90</v>
       </c>
@@ -19979,7 +19973,7 @@
         <v>0.98088888888888903</v>
       </c>
     </row>
-    <row r="467" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A467" s="15" t="s">
         <v>90</v>
       </c>
@@ -20018,7 +20012,7 @@
         <v>1.4726666666666666</v>
       </c>
     </row>
-    <row r="468" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A468" s="15" t="s">
         <v>90</v>
       </c>
@@ -20060,7 +20054,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="469" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A469" s="15" t="s">
         <v>90</v>
       </c>
@@ -20102,7 +20096,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="470" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A470" s="15" t="s">
         <v>90</v>
       </c>
@@ -20144,7 +20138,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="471" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A471" s="17" t="s">
         <v>90</v>
       </c>
@@ -20176,7 +20170,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="472" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A472" s="17" t="s">
         <v>90</v>
       </c>
@@ -20208,7 +20202,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="473" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A473" s="17" t="s">
         <v>90</v>
       </c>
@@ -20240,7 +20234,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="474" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A474" s="15" t="s">
         <v>90</v>
       </c>
@@ -20282,7 +20276,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="475" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A475" s="15" t="s">
         <v>90</v>
       </c>
@@ -20324,7 +20318,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="476" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A476" s="15" t="s">
         <v>90</v>
       </c>
@@ -20366,7 +20360,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="477" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A477" s="15" t="s">
         <v>90</v>
       </c>
@@ -20405,7 +20399,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="478" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A478" s="15" t="s">
         <v>90</v>
       </c>
@@ -20444,7 +20438,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="479" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A479" s="15" t="s">
         <v>90</v>
       </c>
@@ -20483,7 +20477,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="480" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A480" s="15" t="s">
         <v>90</v>
       </c>
@@ -20522,7 +20516,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="481" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A481" s="15" t="s">
         <v>90</v>
       </c>
@@ -20561,7 +20555,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="482" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A482" s="15" t="s">
         <v>90</v>
       </c>
@@ -20600,7 +20594,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="483" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A483" s="15" t="s">
         <v>90</v>
       </c>
@@ -20642,7 +20636,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="484" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A484" s="15" t="s">
         <v>90</v>
       </c>
@@ -20684,7 +20678,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="485" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A485" s="15" t="s">
         <v>90</v>
       </c>
@@ -20726,7 +20720,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="486" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A486" s="15" t="s">
         <v>90</v>
       </c>
@@ -20765,7 +20759,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="487" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A487" s="15" t="s">
         <v>90</v>
       </c>
@@ -20804,7 +20798,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="488" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A488" s="15" t="s">
         <v>90</v>
       </c>
@@ -20960,7 +20954,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="492" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492" s="15" t="s">
         <v>90</v>
       </c>
@@ -20999,7 +20993,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="493" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A493" s="15" t="s">
         <v>90</v>
       </c>
@@ -21038,7 +21032,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="494" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A494" s="15" t="s">
         <v>90</v>
       </c>
@@ -21077,7 +21071,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="495" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A495" s="15" t="s">
         <v>90</v>
       </c>
@@ -21119,7 +21113,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="496" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A496" s="15" t="s">
         <v>90</v>
       </c>
@@ -21161,7 +21155,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="497" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A497" s="15" t="s">
         <v>90</v>
       </c>
@@ -21203,7 +21197,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="498" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A498" s="15" t="s">
         <v>90</v>
       </c>
@@ -21242,7 +21236,7 @@
         <v>0.29842105263157892</v>
       </c>
     </row>
-    <row r="499" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A499" s="15" t="s">
         <v>90</v>
       </c>
@@ -21281,7 +21275,7 @@
         <v>0.46312500000000006</v>
       </c>
     </row>
-    <row r="500" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A500" s="15" t="s">
         <v>90</v>
       </c>
@@ -21320,7 +21314,7 @@
         <v>0.4264705882352941</v>
       </c>
     </row>
-    <row r="501" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A501" s="15" t="s">
         <v>90</v>
       </c>
@@ -21358,7 +21352,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="502" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A502" s="15" t="s">
         <v>90</v>
       </c>
@@ -21396,7 +21390,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="503" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A503" s="15" t="s">
         <v>90</v>
       </c>
@@ -21435,6 +21429,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E503" xr:uid="{91453227-9FB7-42F0-8C4A-4B424D6C8830}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Carrot Juicing"/>
+        <filter val="Carrot Vegetable Fresh"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -21781,6 +21783,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="851a8733-41a3-4250-a9ab-11819fdc6ee0" ContentTypeId="0x0101007A9E73D2CE4B824B95B137B81129B67601" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Document_Status xmlns="8e4dc625-a080-46dd-a669-0042841ac301" xsi:nil="true"/>
+    <PFR_Author xmlns="8e4dc625-a080-46dd-a669-0042841ac301">
+      <UserInfo>
+        <DisplayName>Steven Dellow</DisplayName>
+        <AccountId>26</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </PFR_Author>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="General Report" ma:contentTypeID="0x0101007A9E73D2CE4B824B95B137B81129B67601009C21748F7EF43444A0870BDF043FA6D0" ma:contentTypeVersion="16" ma:contentTypeDescription="Report relating to various topics. May include progress and team reports." ma:contentTypeScope="" ma:versionID="fc328c93d82301f3c79e4382afd79ccb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8e4dc625-a080-46dd-a669-0042841ac301" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bc7f21c5add3fee0d55851afabb3097" ns2:_="">
     <xsd:import namespace="8e4dc625-a080-46dd-a669-0042841ac301"/>
@@ -21929,36 +21960,39 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Document_Status xmlns="8e4dc625-a080-46dd-a669-0042841ac301" xsi:nil="true"/>
-    <PFR_Author xmlns="8e4dc625-a080-46dd-a669-0042841ac301">
-      <UserInfo>
-        <DisplayName>Steven Dellow</DisplayName>
-        <AccountId>26</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </PFR_Author>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1F1626F-5086-4646-961B-C2972B3F9DF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87E9A4E3-A187-4AE2-B6D8-6CA16143045B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="851a8733-41a3-4250-a9ab-11819fdc6ee0" ContentTypeId="0x0101007A9E73D2CE4B824B95B137B81129B67601" PreviousValue="false"/>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B4E57E4-F66A-44AD-9570-5F2D0F35BF1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8e4dc625-a080-46dd-a669-0042841ac301"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB485E88-61DB-4B23-AD23-246E76DBCC44}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21974,36 +22008,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B4E57E4-F66A-44AD-9570-5F2D0F35BF1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8e4dc625-a080-46dd-a669-0042841ac301"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87E9A4E3-A187-4AE2-B6D8-6CA16143045B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1F1626F-5086-4646-961B-C2972B3F9DF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>